<commit_message>
Alteração Planilha de requisitos
</commit_message>
<xml_diff>
--- a/PrototipoRequisitos.xlsx
+++ b/PrototipoRequisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saulooliveira/Desktop/Arte6/arte6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B5EA5-9F8A-8844-A7FB-461062FF8DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E74A344-0B90-484A-A6C7-EDE0EE888AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,6 +147,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1493,7 +1494,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -3157,15 +3158,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T47" xr:uid="{BF830F64-A985-40BC-8F1E-B2AA878BAB5C}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H47" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G47" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Atualização Planilha de requisitos
</commit_message>
<xml_diff>
--- a/PrototipoRequisitos.xlsx
+++ b/PrototipoRequisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saulooliveira/Desktop/Arte6/arte6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo\Desktop\Arte6\arte6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E74A344-0B90-484A-A6C7-EDE0EE888AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBCCC7F-45A9-4978-8265-78A6939C166D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
   <si>
     <t>Solicitante</t>
   </si>
@@ -133,6 +133,48 @@
   </si>
   <si>
     <t>A aplicação deverá ter um cadastro único</t>
+  </si>
+  <si>
+    <t>A aplicação deverá enviar um email confirmando o cadastro do usuário</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>Não Funcional</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Proposto</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Implementado</t>
+  </si>
+  <si>
+    <t>A aplicação exibirá de forma parcial o conteúdo, permitindo a visualização apenas por usuários registrados.</t>
+  </si>
+  <si>
+    <t>00/00/2020</t>
+  </si>
+  <si>
+    <t>A aplicação deverá conter um botão para redirecionar o usuário para o topo da página</t>
+  </si>
+  <si>
+    <t>A aplicação deverá ter um sistema de sessão</t>
   </si>
 </sst>
 </file>
@@ -1490,40 +1532,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:U68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="26.1640625" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="39.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="39.1640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="16" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.1640625" style="1"/>
+    <col min="19" max="19" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="2" customFormat="1" ht="29" thickBot="1">
+    <row r="1" spans="2:21" s="2" customFormat="1" ht="27.75" thickBot="1">
       <c r="B1" s="10" t="s">
         <v>18</v>
       </c>
@@ -1583,17 +1625,25 @@
       </c>
       <c r="U1" s="9"/>
     </row>
-    <row r="2" spans="2:21" s="3" customFormat="1" ht="28">
+    <row r="2" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B2" s="14">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5">
+        <v>100</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1601,24 +1651,36 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="6"/>
+      <c r="O2" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
-      <c r="T2" s="16"/>
-    </row>
-    <row r="3" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T2" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" s="3" customFormat="1" ht="41.25" thickBot="1">
       <c r="B3" s="15">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="5">
+        <v>75</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1626,24 +1688,36 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="2:21" s="3" customFormat="1" ht="42">
+      <c r="T3" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" s="3" customFormat="1" ht="54.75" thickBot="1">
       <c r="B4" s="14">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="5">
+        <v>75</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1651,24 +1725,36 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T4" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B5" s="15">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5">
+        <v>75</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1676,24 +1762,36 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T5" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B6" s="14">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5">
+        <v>75</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1701,49 +1799,79 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T6" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B7" s="15">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5">
+        <v>100</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="O7" s="6">
+        <v>43874</v>
+      </c>
+      <c r="P7" s="6">
+        <v>43882</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-    </row>
-    <row r="8" spans="2:21" s="3" customFormat="1" ht="15">
+      <c r="T7" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B8" s="14">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5">
+        <v>100</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1751,24 +1879,36 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="2:21" s="3" customFormat="1" ht="15">
+      <c r="T8" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B9" s="15">
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5">
+        <v>100</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -1776,24 +1916,36 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
+      <c r="O9" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T9" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B10" s="14">
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1801,24 +1953,36 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T10" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="3" customFormat="1" ht="41.25" thickBot="1">
       <c r="B11" s="15">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="5">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1826,24 +1990,36 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="6"/>
+      <c r="O11" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T11" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="3" customFormat="1" ht="41.25" thickBot="1">
       <c r="B12" s="14">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5">
+        <v>100</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1851,24 +2027,36 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="O12" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T12" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B13" s="15">
         <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5">
+        <v>100</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1876,24 +2064,36 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
+      <c r="O13" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="2:21" s="3" customFormat="1" ht="15">
+      <c r="T13" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B14" s="14">
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="5">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1901,24 +2101,36 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
+      <c r="O14" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T14" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B15" s="15">
         <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="5">
+        <v>75</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1926,24 +2138,36 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
+      <c r="O15" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="2:21" s="3" customFormat="1" ht="28">
+      <c r="T15" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B16" s="14">
         <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="5">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1951,24 +2175,36 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
+      <c r="O16" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T16" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" s="3" customFormat="1" ht="27.75" thickBot="1">
       <c r="B17" s="15">
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="5">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1976,22 +2212,36 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
+      <c r="O17" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T17" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" s="3" customFormat="1" ht="40.5">
       <c r="B18" s="14">
         <v>17</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="5">
+        <v>75</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1999,22 +2249,36 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
+      <c r="O18" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T18" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" s="3" customFormat="1" ht="54">
       <c r="B19" s="15">
         <v>18</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="5">
+        <v>75</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -2022,22 +2286,36 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
+      <c r="O19" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" s="3" customFormat="1" ht="40.5">
       <c r="B20" s="14">
         <v>19</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5">
+        <v>100</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -2045,37 +2323,61 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
+      <c r="O20" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T20" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" s="3" customFormat="1" ht="27">
       <c r="B21" s="15">
         <v>20</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="5">
+        <v>100</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
+      <c r="O21" s="6">
+        <v>43891</v>
+      </c>
+      <c r="P21" s="6">
+        <v>43891</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="2:20" s="3" customFormat="1" ht="15">
+      <c r="T21" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B22" s="14">
         <v>21</v>
       </c>
@@ -2098,7 +2400,7 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="23" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B23" s="15">
         <v>22</v>
       </c>
@@ -2121,7 +2423,7 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="24" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B24" s="14">
         <v>23</v>
       </c>
@@ -2144,7 +2446,7 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="25" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B25" s="15">
         <v>24</v>
       </c>
@@ -2167,7 +2469,7 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="26" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B26" s="14">
         <v>25</v>
       </c>
@@ -2190,7 +2492,7 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
     </row>
-    <row r="27" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="27" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B27" s="15">
         <v>26</v>
       </c>
@@ -2213,7 +2515,7 @@
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="28" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B28" s="14">
         <v>27</v>
       </c>
@@ -2236,7 +2538,7 @@
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
     </row>
-    <row r="29" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="29" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B29" s="15">
         <v>28</v>
       </c>
@@ -2259,7 +2561,7 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="30" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B30" s="14">
         <v>29</v>
       </c>
@@ -2282,7 +2584,7 @@
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="31" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B31" s="15">
         <v>30</v>
       </c>
@@ -2305,7 +2607,7 @@
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
     </row>
-    <row r="32" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="32" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B32" s="14">
         <v>31</v>
       </c>
@@ -2328,7 +2630,7 @@
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="33" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B33" s="15">
         <v>32</v>
       </c>
@@ -2351,7 +2653,7 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
     </row>
-    <row r="34" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="34" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B34" s="14">
         <v>33</v>
       </c>
@@ -2374,7 +2676,7 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="35" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B35" s="15">
         <v>34</v>
       </c>
@@ -2397,7 +2699,7 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
     </row>
-    <row r="36" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="36" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B36" s="14">
         <v>35</v>
       </c>
@@ -2420,7 +2722,7 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="37" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B37" s="15">
         <v>36</v>
       </c>
@@ -2443,7 +2745,7 @@
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="38" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B38" s="14">
         <v>37</v>
       </c>
@@ -2466,7 +2768,7 @@
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
     </row>
-    <row r="39" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="39" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B39" s="15">
         <v>38</v>
       </c>
@@ -2489,7 +2791,7 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="40" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B40" s="14">
         <v>39</v>
       </c>
@@ -2512,7 +2814,7 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="41" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B41" s="15">
         <v>40</v>
       </c>
@@ -2535,7 +2837,7 @@
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="42" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B42" s="14">
         <v>41</v>
       </c>
@@ -2558,7 +2860,7 @@
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="43" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B43" s="15">
         <v>42</v>
       </c>
@@ -2581,7 +2883,7 @@
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="44" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B44" s="14">
         <v>43</v>
       </c>
@@ -2604,7 +2906,7 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
     </row>
-    <row r="45" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="45" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B45" s="15">
         <v>44</v>
       </c>
@@ -2627,7 +2929,7 @@
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
     </row>
-    <row r="46" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="46" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B46" s="14">
         <v>45</v>
       </c>
@@ -2650,7 +2952,7 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="47" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B47" s="15">
         <v>46</v>
       </c>
@@ -2673,7 +2975,7 @@
       <c r="S47" s="7"/>
       <c r="T47" s="5"/>
     </row>
-    <row r="48" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="48" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B48" s="14">
         <v>47</v>
       </c>
@@ -2696,7 +2998,7 @@
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
     </row>
-    <row r="49" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="49" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B49" s="15">
         <v>48</v>
       </c>
@@ -2719,7 +3021,7 @@
       <c r="S49" s="7"/>
       <c r="T49" s="7"/>
     </row>
-    <row r="50" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="50" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B50" s="14">
         <v>49</v>
       </c>
@@ -2742,7 +3044,7 @@
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
     </row>
-    <row r="51" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="51" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B51" s="15">
         <v>50</v>
       </c>
@@ -2765,7 +3067,7 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
     </row>
-    <row r="52" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="52" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B52" s="14">
         <v>51</v>
       </c>
@@ -2788,7 +3090,7 @@
       <c r="S52" s="7"/>
       <c r="T52" s="7"/>
     </row>
-    <row r="53" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="53" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B53" s="15">
         <v>52</v>
       </c>
@@ -2811,7 +3113,7 @@
       <c r="S53" s="7"/>
       <c r="T53" s="7"/>
     </row>
-    <row r="54" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="54" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B54" s="14">
         <v>53</v>
       </c>
@@ -2834,7 +3136,7 @@
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
     </row>
-    <row r="55" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="55" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B55" s="15">
         <v>54</v>
       </c>
@@ -2857,7 +3159,7 @@
       <c r="S55" s="7"/>
       <c r="T55" s="7"/>
     </row>
-    <row r="56" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="56" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B56" s="14">
         <v>55</v>
       </c>
@@ -2880,7 +3182,7 @@
       <c r="S56" s="7"/>
       <c r="T56" s="7"/>
     </row>
-    <row r="57" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="57" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B57" s="15">
         <v>56</v>
       </c>
@@ -2903,7 +3205,7 @@
       <c r="S57" s="7"/>
       <c r="T57" s="7"/>
     </row>
-    <row r="58" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="58" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B58" s="14">
         <v>57</v>
       </c>
@@ -2926,7 +3228,7 @@
       <c r="S58" s="7"/>
       <c r="T58" s="7"/>
     </row>
-    <row r="59" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="59" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B59" s="15">
         <v>58</v>
       </c>
@@ -2949,7 +3251,7 @@
       <c r="S59" s="7"/>
       <c r="T59" s="7"/>
     </row>
-    <row r="60" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="60" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B60" s="14">
         <v>59</v>
       </c>
@@ -2972,7 +3274,7 @@
       <c r="S60" s="7"/>
       <c r="T60" s="7"/>
     </row>
-    <row r="61" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="61" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B61" s="15">
         <v>60</v>
       </c>
@@ -2995,7 +3297,7 @@
       <c r="S61" s="7"/>
       <c r="T61" s="7"/>
     </row>
-    <row r="62" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="62" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B62" s="14">
         <v>61</v>
       </c>
@@ -3018,7 +3320,7 @@
       <c r="S62" s="7"/>
       <c r="T62" s="7"/>
     </row>
-    <row r="63" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="63" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B63" s="15">
         <v>62</v>
       </c>
@@ -3041,7 +3343,7 @@
       <c r="S63" s="7"/>
       <c r="T63" s="7"/>
     </row>
-    <row r="64" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="64" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B64" s="14">
         <v>63</v>
       </c>
@@ -3064,7 +3366,7 @@
       <c r="S64" s="7"/>
       <c r="T64" s="7"/>
     </row>
-    <row r="65" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="65" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B65" s="15">
         <v>64</v>
       </c>
@@ -3087,7 +3389,7 @@
       <c r="S65" s="7"/>
       <c r="T65" s="7"/>
     </row>
-    <row r="66" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="66" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B66" s="14">
         <v>65</v>
       </c>
@@ -3110,7 +3412,7 @@
       <c r="S66" s="7"/>
       <c r="T66" s="7"/>
     </row>
-    <row r="67" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="67" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B67" s="15">
         <v>66</v>
       </c>
@@ -3133,7 +3435,7 @@
       <c r="S67" s="7"/>
       <c r="T67" s="7"/>
     </row>
-    <row r="68" spans="2:20" s="3" customFormat="1" ht="15">
+    <row r="68" spans="2:20" s="3" customFormat="1" ht="15.75">
       <c r="B68" s="14">
         <v>67</v>
       </c>

</xml_diff>